<commit_message>
some updates to analyses and workflow
</commit_message>
<xml_diff>
--- a/outputs/concern_thresh.xlsx
+++ b/outputs/concern_thresh.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -410,6 +410,26 @@
         <v>0.6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2023</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>0.26</v>
+      </c>
+      <c r="D3">
+        <v>0.38</v>
+      </c>
+      <c r="E3">
+        <v>0.49</v>
+      </c>
+      <c r="F3">
+        <v>0.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -417,7 +437,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -459,6 +479,20 @@
         <v>0.52</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2023</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>0.34</v>
+      </c>
+      <c r="D3">
+        <v>0.52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
keeping threshold definitions fixed for one whole year, updating concern classification monthly based on that
</commit_message>
<xml_diff>
--- a/outputs/concern_thresh.xlsx
+++ b/outputs/concern_thresh.xlsx
@@ -1,22 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCI\dark-loci\outputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25BF1A8-6CF5-44F0-9E35-688DBDC94089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINE" sheetId="1" r:id="rId1"/>
     <sheet name="COARSE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>THRESH.FINE1</t>
+  </si>
+  <si>
+    <t>THRESH.FINE2</t>
+  </si>
+  <si>
+    <t>THRESH.FINE3</t>
+  </si>
+  <si>
+    <t>THRESH.FINE4</t>
+  </si>
+  <si>
+    <t>THRESH.COARSE1</t>
+  </si>
+  <si>
+    <t>THRESH.COARSE2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +99,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -110,7 +153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +185,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +237,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,46 +430,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>YEAR</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>MONTH</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>THRESH.FINE1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>THRESH.FINE2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>THRESH.FINE3</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>THRESH.FINE4</t>
-        </is>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -408,26 +477,6 @@
       </c>
       <c r="F2">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2023</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>0.25</v>
-      </c>
-      <c r="D3">
-        <v>0.37</v>
-      </c>
-      <c r="E3">
-        <v>0.47</v>
-      </c>
-      <c r="F3">
-        <v>0.57</v>
       </c>
     </row>
   </sheetData>
@@ -436,36 +485,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>YEAR</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>MONTH</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>THRESH.COARSE1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>THRESH.COARSE2</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -477,20 +520,6 @@
       </c>
       <c r="D2">
         <v>0.52</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2023</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>0.34</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with yearly calculation
</commit_message>
<xml_diff>
--- a/outputs/concern_thresh.xlsx
+++ b/outputs/concern_thresh.xlsx
@@ -1,57 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCI\dark-loci\outputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25BF1A8-6CF5-44F0-9E35-688DBDC94089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="FINE" sheetId="1" r:id="rId1"/>
     <sheet name="COARSE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>YEAR</t>
-  </si>
-  <si>
-    <t>MONTH</t>
-  </si>
-  <si>
-    <t>THRESH.FINE1</t>
-  </si>
-  <si>
-    <t>THRESH.FINE2</t>
-  </si>
-  <si>
-    <t>THRESH.FINE3</t>
-  </si>
-  <si>
-    <t>THRESH.FINE4</t>
-  </si>
-  <si>
-    <t>THRESH.COARSE1</t>
-  </si>
-  <si>
-    <t>THRESH.COARSE2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,25 +56,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -153,7 +114,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,27 +146,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,24 +180,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,36 +355,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>YEAR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>MONTH</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>THRESH.FINE1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>THRESH.FINE2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>THRESH.FINE3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>THRESH.FINE4</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -477,6 +420,32 @@
       </c>
       <c r="F2">
         <v>0.6</v>
+      </c>
+      <c r="G2" s="2">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2024</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0.34</v>
+      </c>
+      <c r="D3">
+        <v>0.46</v>
+      </c>
+      <c r="E3">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.65</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45352</v>
       </c>
     </row>
   </sheetData>
@@ -485,30 +454,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="20.7109375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>YEAR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>MONTH</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>THRESH.COARSE1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>THRESH.COARSE2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -520,6 +503,26 @@
       </c>
       <c r="D2">
         <v>0.52</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2024</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0.43</v>
+      </c>
+      <c r="D3">
+        <v>0.59</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>